<commit_message>
testin changes from 3/16
</commit_message>
<xml_diff>
--- a/Auto Instrumentation Sheet.xlsx
+++ b/Auto Instrumentation Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MASA-Avionics\masa-umich\mcnugget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0B7C5A-D889-449A-B5A1-C8B7A94890B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E6CD8A-F437-44BA-A2F9-45BB40355BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -612,8 +612,8 @@
   </sheetPr>
   <dimension ref="A1:Y90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="N12" workbookViewId="0">
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>